<commit_message>
lettertest wordt voltooid en uitgevoerd. Opgeslagen in excel
</commit_message>
<xml_diff>
--- a/backend/Data/data.xlsx
+++ b/backend/Data/data.xlsx
@@ -465,22 +465,22 @@
         <v>test</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>1000</v>
+        <v>120</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1000</v>
+        <v>120</v>
       </c>
       <c r="F3">
-        <v>300</v>
+        <v>10</v>
       </c>
       <c r="G3">
-        <v>500</v>
+        <v>110</v>
       </c>
       <c r="H3">
         <v>0.05</v>

</xml_diff>

<commit_message>
mogelijkheid om groepen actief te zetten, er kan telkens maar 1 groep actief zijn
</commit_message>
<xml_diff>
--- a/backend/Data/data.xlsx
+++ b/backend/Data/data.xlsx
@@ -457,7 +457,7 @@
         <v>0.01</v>
       </c>
       <c r="I2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -486,7 +486,7 @@
         <v>0.05</v>
       </c>
       <c r="I3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new groups can now be created
</commit_message>
<xml_diff>
--- a/backend/Data/data.xlsx
+++ b/backend/Data/data.xlsx
@@ -1,41 +1,65 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bvdv\bvdv-app\backend\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAA3611-2103-41E5-9168-AA1D144EBFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Groep</t>
+  </si>
+  <si>
+    <t>Aantal_deelnemers</t>
+  </si>
+  <si>
+    <t>Aantal_letterparen_naam</t>
+  </si>
+  <si>
+    <t>Aantal_letterparen_dummy</t>
+  </si>
+  <si>
+    <t>Totaal_letterparen</t>
+  </si>
+  <si>
+    <t>Aantal_eigen_letters_verworpen</t>
+  </si>
+  <si>
+    <t>Aantal_vreemde_letters_verworpen</t>
+  </si>
+  <si>
+    <t>Significantie</t>
+  </si>
+  <si>
+    <t>Actief</t>
+  </si>
+  <si>
+    <t>Totaal</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -65,13 +89,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,44 +428,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Groep</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Aantal_deelnemers</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Aantal_letterparen_naam</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Aantal_letterparen_dummy</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Totaal_letterparen</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Aantal_eigen_letters_verworpen</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Aantal_vreemde_letters_verworpen</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Significantie</v>
-      </c>
-      <c r="I1" t="str">
-        <v>Actief</v>
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Totaal</v>
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
       </c>
       <c r="B2">
         <v>908</v>
@@ -457,12 +492,12 @@
         <v>0.01</v>
       </c>
       <c r="I2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>test</v>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
       </c>
       <c r="B3">
         <v>12</v>
@@ -486,12 +521,18 @@
         <v>0.05</v>
       </c>
       <c r="I3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I3"/>
+    <ignoredError sqref="A1:I3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
groepen kunnen worden verwijderd
</commit_message>
<xml_diff>
--- a/backend/Data/data.xlsx
+++ b/backend/Data/data.xlsx
@@ -1,65 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bvdv\bvdv-app\backend\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAA3611-2103-41E5-9168-AA1D144EBFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Groep</t>
-  </si>
-  <si>
-    <t>Aantal_deelnemers</t>
-  </si>
-  <si>
-    <t>Aantal_letterparen_naam</t>
-  </si>
-  <si>
-    <t>Aantal_letterparen_dummy</t>
-  </si>
-  <si>
-    <t>Totaal_letterparen</t>
-  </si>
-  <si>
-    <t>Aantal_eigen_letters_verworpen</t>
-  </si>
-  <si>
-    <t>Aantal_vreemde_letters_verworpen</t>
-  </si>
-  <si>
-    <t>Significantie</t>
-  </si>
-  <si>
-    <t>Actief</t>
-  </si>
-  <si>
-    <t>Totaal</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -89,21 +65,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -428,47 +396,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Groep</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Aantal_deelnemers</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Aantal_letterparen_naam</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Aantal_letterparen_dummy</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Totaal_letterparen</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Aantal_eigen_letters_verworpen</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Aantal_vreemde_letters_verworpen</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Significantie</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Actief</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Totaal</v>
       </c>
       <c r="B2">
         <v>908</v>
@@ -492,12 +457,12 @@
         <v>0.01</v>
       </c>
       <c r="I2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>test</v>
       </c>
       <c r="B3">
         <v>12</v>
@@ -521,18 +486,12 @@
         <v>0.05</v>
       </c>
       <c r="I3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:I3" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bugfix for backend of the test
</commit_message>
<xml_diff>
--- a/backend/Data/data.xlsx
+++ b/backend/Data/data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -436,28 +436,28 @@
         <v>Totaal</v>
       </c>
       <c r="B2">
-        <v>908</v>
+        <v>919</v>
       </c>
       <c r="C2">
-        <v>9080</v>
+        <v>9160</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E2">
-        <v>9080</v>
+        <v>9190</v>
       </c>
       <c r="F2">
-        <v>2952</v>
+        <v>2969</v>
       </c>
       <c r="G2">
-        <v>5140</v>
+        <v>5223</v>
       </c>
       <c r="H2">
         <v>0.01</v>
       </c>
       <c r="I2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -489,9 +489,38 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>test lokaal</v>
+      </c>
+      <c r="B4">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>80</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="E4">
+        <v>110</v>
+      </c>
+      <c r="F4">
+        <v>17</v>
+      </c>
+      <c r="G4">
+        <v>83</v>
+      </c>
+      <c r="H4">
+        <v>0.05</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor test en chart naar 1 pagina. methodes en visuals rond actieve groep weg, select groep ook voor nederlands
</commit_message>
<xml_diff>
--- a/backend/Data/data.xlsx
+++ b/backend/Data/data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -436,19 +436,19 @@
         <v>Totaal</v>
       </c>
       <c r="B2">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="C2">
-        <v>9160</v>
+        <v>9176</v>
       </c>
       <c r="D2">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E2">
-        <v>9190</v>
+        <v>9210</v>
       </c>
       <c r="F2">
-        <v>2969</v>
+        <v>2985</v>
       </c>
       <c r="G2">
         <v>5223</v>
@@ -515,12 +515,41 @@
         <v>0.05</v>
       </c>
       <c r="I4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>live</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>16</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0.05</v>
+      </c>
+      <c r="I5" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
delete group gefixt, kleuren letter selectie engels aangepast, talen switchbaar, bg knoppen aangepast
</commit_message>
<xml_diff>
--- a/backend/Data/data.xlsx
+++ b/backend/Data/data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -436,22 +436,22 @@
         <v>Totaal</v>
       </c>
       <c r="B2">
-        <v>921</v>
+        <v>924</v>
       </c>
       <c r="C2">
-        <v>9176</v>
+        <v>9199</v>
       </c>
       <c r="D2">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E2">
-        <v>9210</v>
+        <v>9240</v>
       </c>
       <c r="F2">
-        <v>2985</v>
+        <v>2991</v>
       </c>
       <c r="G2">
-        <v>5223</v>
+        <v>5240</v>
       </c>
       <c r="H2">
         <v>0.01</v>
@@ -491,65 +491,36 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>test lokaal</v>
+        <v>pre-meeting</v>
       </c>
       <c r="B4">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>80</v>
+        <v>23</v>
       </c>
       <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4">
         <v>30</v>
       </c>
-      <c r="E4">
-        <v>110</v>
-      </c>
       <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
         <v>17</v>
-      </c>
-      <c r="G4">
-        <v>83</v>
       </c>
       <c r="H4">
         <v>0.05</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>live</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>16</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>20</v>
-      </c>
-      <c r="F5">
-        <v>16</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0.05</v>
-      </c>
-      <c r="I5" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
after test completion, the window dissapears and a confirmation message is shown for 3 seconds.
</commit_message>
<xml_diff>
--- a/backend/Data/data.xlsx
+++ b/backend/Data/data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -436,22 +436,22 @@
         <v>Totaal</v>
       </c>
       <c r="B2">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="C2">
-        <v>9239</v>
+        <v>9247</v>
       </c>
       <c r="D2">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E2">
-        <v>9320</v>
+        <v>9330</v>
       </c>
       <c r="F2">
-        <v>3004</v>
+        <v>3008</v>
       </c>
       <c r="G2">
-        <v>5267</v>
+        <v>5271</v>
       </c>
       <c r="H2">
         <v>0.01</v>
@@ -489,9 +489,38 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>test-feedback</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>0.05</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
implementatie significantie ratio based
</commit_message>
<xml_diff>
--- a/backend/Data/data.xlsx
+++ b/backend/Data/data.xlsx
@@ -1,41 +1,65 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bvdv\bvdv-app\backend\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61B05A3-8AD8-4A91-8E2F-3F1089CECF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="780" yWindow="-15420" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Groep</t>
+  </si>
+  <si>
+    <t>Aantal_deelnemers</t>
+  </si>
+  <si>
+    <t>Aantal_letterparen_naam</t>
+  </si>
+  <si>
+    <t>Aantal_letterparen_dummy</t>
+  </si>
+  <si>
+    <t>Totaal_letterparen</t>
+  </si>
+  <si>
+    <t>Aantal_eigen_letters_verworpen</t>
+  </si>
+  <si>
+    <t>Aantal_vreemde_letters_verworpen</t>
+  </si>
+  <si>
+    <t>Significantie</t>
+  </si>
+  <si>
+    <t>Actief</t>
+  </si>
+  <si>
+    <t>Totaal</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -65,13 +89,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,62 +428,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Groep</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Aantal_deelnemers</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Aantal_letterparen_naam</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Aantal_letterparen_dummy</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Totaal_letterparen</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Aantal_eigen_letters_verworpen</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Aantal_vreemde_letters_verworpen</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Significantie</v>
-      </c>
-      <c r="I1" t="str">
-        <v>Actief</v>
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Totaal</v>
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>935</v>
+        <v>908</v>
       </c>
       <c r="C2">
-        <v>9263</v>
+        <v>8092</v>
       </c>
       <c r="D2">
-        <v>87</v>
+        <v>988</v>
       </c>
       <c r="E2">
-        <v>9350</v>
+        <v>9080</v>
       </c>
       <c r="F2">
-        <v>3011</v>
+        <v>2952</v>
       </c>
       <c r="G2">
-        <v>5284</v>
+        <v>5140</v>
       </c>
       <c r="H2">
         <v>0.01</v>
@@ -460,67 +506,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>test</v>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="I3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>test-feedback</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>24</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>30</v>
-      </c>
-      <c r="F4">
-        <v>7</v>
-      </c>
-      <c r="G4">
-        <v>17</v>
-      </c>
-      <c r="H4">
-        <v>0.05</v>
-      </c>
-      <c r="I4" t="b">
-        <v>0</v>
-      </c>
-    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I4"/>
+    <ignoredError sqref="A1:I1 A2 H2:I2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change request toon, lettertest op aparte pagina, enkel engelstalige paginas
</commit_message>
<xml_diff>
--- a/backend/Data/data.xlsx
+++ b/backend/Data/data.xlsx
@@ -1,65 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bvdv\bvdv-app\backend\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61B05A3-8AD8-4A91-8E2F-3F1089CECF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="780" yWindow="-15420" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Groep</t>
-  </si>
-  <si>
-    <t>Aantal_deelnemers</t>
-  </si>
-  <si>
-    <t>Aantal_letterparen_naam</t>
-  </si>
-  <si>
-    <t>Aantal_letterparen_dummy</t>
-  </si>
-  <si>
-    <t>Totaal_letterparen</t>
-  </si>
-  <si>
-    <t>Aantal_eigen_letters_verworpen</t>
-  </si>
-  <si>
-    <t>Aantal_vreemde_letters_verworpen</t>
-  </si>
-  <si>
-    <t>Significantie</t>
-  </si>
-  <si>
-    <t>Actief</t>
-  </si>
-  <si>
-    <t>Totaal</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -89,21 +65,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -428,76 +396,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Groep</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Aantal_deelnemers</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Aantal_letterparen_naam</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Aantal_letterparen_dummy</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Totaal_letterparen</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Aantal_eigen_letters_verworpen</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Aantal_vreemde_letters_verworpen</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Significantie</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Actief</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Totaal</v>
       </c>
       <c r="B2">
-        <v>908</v>
+        <v>911</v>
       </c>
       <c r="C2">
-        <v>8092</v>
+        <v>8108</v>
       </c>
       <c r="D2">
-        <v>988</v>
+        <v>1002</v>
       </c>
       <c r="E2">
-        <v>9080</v>
+        <v>9110</v>
       </c>
       <c r="F2">
-        <v>2952</v>
+        <v>2959</v>
       </c>
       <c r="G2">
-        <v>5140</v>
+        <v>5149</v>
       </c>
       <c r="H2">
         <v>0.01</v>
@@ -506,9 +460,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Test</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -535,12 +489,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Elia NL</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>30</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+      <c r="G4">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>0.05</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Elia FR</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0.05</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:I1 A2 H2:I2" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>